<commit_message>
Queue name changed to its original name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GSHANM1\Uipath_code\REFRAMEWORK-RPABOT11\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59E3F08-D117-4AE8-AD62-27147BE5B90A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DD0464-AD00-4330-812D-AE5E9C0D41B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>Static part of logging message. Calling Get Transaction Data.</t>
   </si>
   <si>
-    <t>test2</t>
-  </si>
-  <si>
     <t>Data Source=itgc2w000006\ngc_od_prod;Initial Catalog=eSPSv14OD_PROD;Integrated Security=True</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Con_QA</t>
+  </si>
+  <si>
+    <t>RPABOT11-ODAS-NGC-POEXTRACT</t>
   </si>
 </sst>
 </file>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -558,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -1580,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1707,18 +1707,18 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>